<commit_message>
Update class and character
</commit_message>
<xml_diff>
--- a/Datas/Defines/__beans__.xlsx
+++ b/Datas/Defines/__beans__.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\SunHeSLGConfigs\Datas\Defines\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E32E321-8F1A-4585-9F51-94BCADC85A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9371EE43-B577-41E9-9C7C-C1D643E92A60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,11 +17,11 @@
   </sheets>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Claymore - Personal View" guid="{CB89C7C3-9291-4D1D-ABF6-F72D75238F47}" mergeInterval="0" personalView="1" maximized="1" xWindow="-1608" yWindow="-8" windowWidth="1616" windowHeight="868" activeSheetId="1"/>
+    <customWorkbookView name="施逸诗 - 个人视图" guid="{03E8AAD4-4054-43A1-B504-82AC2A8AAC3D}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="王树湃 - 个人视图" guid="{BEB32F08-F073-4C54-AB58-82CE415D5183}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1048" activeSheetId="1"/>
+    <customWorkbookView name="相钰 - 个人视图" guid="{A139AFD5-47BE-4E02-BD03-EC36313C3819}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
     <customWorkbookView name="李翔 - 个人视图" guid="{086FD590-A994-4456-BE22-C66B2EE54603}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="403" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="相钰 - 个人视图" guid="{A139AFD5-47BE-4E02-BD03-EC36313C3819}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="王树湃 - 个人视图" guid="{BEB32F08-F073-4C54-AB58-82CE415D5183}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1048" activeSheetId="1"/>
-    <customWorkbookView name="施逸诗 - 个人视图" guid="{03E8AAD4-4054-43A1-B504-82AC2A8AAC3D}" mergeInterval="0" personalView="1" maximized="1" xWindow="1912" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="Claymore - Personal View" guid="{CB89C7C3-9291-4D1D-ABF6-F72D75238F47}" mergeInterval="0" personalView="1" maximized="1" xWindow="-1608" yWindow="-8" windowWidth="1616" windowHeight="868" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>##var</t>
   </si>
@@ -92,12 +92,6 @@
   </si>
   <si>
     <t>注释</t>
-  </si>
-  <si>
-    <t>Movement</t>
-  </si>
-  <si>
-    <t>Mov</t>
   </si>
   <si>
     <t>Build</t>
@@ -557,7 +551,7 @@
   <dimension ref="A1:Q73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F13" sqref="F13:P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -652,20 +646,20 @@
     <row r="4" spans="1:17">
       <c r="A4" s="5"/>
       <c r="B4" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="H4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" t="s">
         <v>37</v>
       </c>
-      <c r="I4" t="s">
-        <v>39</v>
-      </c>
       <c r="K4" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -676,13 +670,13 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="H5" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -693,13 +687,13 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="H6" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -710,13 +704,13 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="H7" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -727,13 +721,13 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="H8" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -744,13 +738,13 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="H9" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K9" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -761,13 +755,13 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="H10" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K10" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -778,13 +772,13 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="H11" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K11" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -795,13 +789,13 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="H12" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K12" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -811,15 +805,8 @@
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="H13" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" t="s">
-        <v>39</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="H13" s="6"/>
+      <c r="K13" s="5"/>
     </row>
     <row r="14" spans="1:17">
       <c r="H14" s="2"/>
@@ -1153,13 +1140,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{086FD590-A994-4456-BE22-C66B2EE54603}" topLeftCell="A25">
-      <selection activeCell="F32" sqref="F32"/>
+    <customSheetView guid="{CB89C7C3-9291-4D1D-ABF6-F72D75238F47}">
+      <selection activeCell="K7" sqref="K7"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{A139AFD5-47BE-4E02-BD03-EC36313C3819}">
-      <selection activeCell="F21" sqref="F21"/>
+    <customSheetView guid="{03E8AAD4-4054-43A1-B504-82AC2A8AAC3D}" topLeftCell="A40">
+      <selection activeCell="I66" sqref="I66"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -1168,13 +1155,13 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{03E8AAD4-4054-43A1-B504-82AC2A8AAC3D}" topLeftCell="A40">
-      <selection activeCell="I66" sqref="I66"/>
+    <customSheetView guid="{A139AFD5-47BE-4E02-BD03-EC36313C3819}">
+      <selection activeCell="F21" sqref="F21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{CB89C7C3-9291-4D1D-ABF6-F72D75238F47}">
-      <selection activeCell="K7" sqref="K7"/>
+    <customSheetView guid="{086FD590-A994-4456-BE22-C66B2EE54603}" topLeftCell="A25">
+      <selection activeCell="F32" sqref="F32"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
     </customSheetView>

</xml_diff>